<commit_message>
to redo offline sensitivity analysis
</commit_message>
<xml_diff>
--- a/A_prepost_processing/IDFs_Sensitivity.xlsx
+++ b/A_prepost_processing/IDFs_Sensitivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wulic\Documents\GitHub\urban_climate_and_who\A_prepost_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35670EE2-9930-441F-8BDD-2195F8AF0DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014EABB4-E579-42E6-924C-7C9B767B8626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cvrmse_energy" sheetId="4" r:id="rId1"/>
@@ -1083,16 +1083,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1444,12 +1444,13 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>